<commit_message>
remove insert_backload and edit excel
</commit_message>
<xml_diff>
--- a/scheduler_agent/excel.xlsx
+++ b/scheduler_agent/excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Bootstrap\scheduler_agent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5DA892E-4DE2-4E55-9AAC-65C538841BE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D202A1-3B72-4243-B842-4A5360A9600D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6D1051C5-B5E8-4EE7-A59A-03C093F1694F}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Customer</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>Troca de modem</t>
-  </si>
-  <si>
-    <t>None</t>
   </si>
 </sst>
 </file>
@@ -453,10 +450,14 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D2" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -482,9 +483,7 @@
       <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -496,6 +495,7 @@
       <c r="C3" t="s">
         <v>16</v>
       </c>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -507,9 +507,7 @@
       <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -533,9 +531,7 @@
       <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -547,9 +543,7 @@
       <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
+      <c r="D7" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>